<commit_message>
added reference date and first interventions
</commit_message>
<xml_diff>
--- a/Supplement_1_-_data_summary.xlsx
+++ b/Supplement_1_-_data_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t xml:space="preserve">BCG atlas</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference date (100 cases)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First national non-pharmaceutical interventions (except borders)</t>
   </si>
   <si>
     <t xml:space="preserve">Algeria</t>
@@ -257,14 +263,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,6 +294,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -296,9 +305,16 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
       <top/>
       <bottom/>
@@ -330,7 +346,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,7 +355,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,6 +377,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -371,37 +411,37 @@
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF2" activeCellId="0" sqref="AF2"/>
+      <selection pane="bottomRight" activeCell="AI11" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.41"/>
@@ -412,127 +452,145 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="12.32"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD1" s="2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="AD1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AMC1" s="3"/>
-      <c r="AMD1" s="3"/>
-      <c r="AME1" s="3"/>
-      <c r="AMF1" s="3"/>
-      <c r="AMG1" s="3"/>
-      <c r="AMH1" s="3"/>
-      <c r="AMI1" s="3"/>
-      <c r="AMJ1" s="3"/>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="71.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="5"/>
+      <c r="AMC1" s="6"/>
+      <c r="AMD1" s="6"/>
+      <c r="AME1" s="6"/>
+      <c r="AMF1" s="6"/>
+      <c r="AMG1" s="6"/>
+      <c r="AMH1" s="6"/>
+      <c r="AMI1" s="6"/>
+      <c r="AMJ1" s="6"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="AH2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
@@ -545,7 +603,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -616,10 +674,16 @@
       <c r="AG3" s="0" t="n">
         <v>23915.7376</v>
       </c>
+      <c r="AH3" s="9" t="n">
+        <v>43911</v>
+      </c>
+      <c r="AI3" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -702,10 +766,16 @@
       <c r="AG4" s="0" t="n">
         <v>2.135</v>
       </c>
+      <c r="AH4" s="9" t="n">
+        <v>43898</v>
+      </c>
+      <c r="AI4" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -788,10 +858,16 @@
       <c r="AG5" s="0" t="n">
         <v>2838.2347</v>
       </c>
+      <c r="AH5" s="9" t="n">
+        <v>43896</v>
+      </c>
+      <c r="AI5" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -874,10 +950,16 @@
       <c r="AC6" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="AH6" s="9" t="n">
+        <v>43903</v>
+      </c>
+      <c r="AI6" s="10" t="n">
+        <v>43903</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -936,10 +1018,16 @@
       <c r="AC7" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH7" s="9" t="n">
+        <v>43905</v>
+      </c>
+      <c r="AI7" s="10" t="n">
+        <v>43904</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -998,10 +1086,16 @@
       <c r="AC8" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH8" s="9" t="n">
+        <v>43909</v>
+      </c>
+      <c r="AI8" s="10" t="n">
+        <v>43901</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -1066,7 +1160,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -1134,10 +1228,16 @@
       <c r="AC10" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH10" s="9" t="n">
+        <v>43909</v>
+      </c>
+      <c r="AI10" s="10" t="n">
+        <v>43899</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -1220,10 +1320,16 @@
       <c r="AG11" s="0" t="n">
         <v>40609.4029</v>
       </c>
+      <c r="AH11" s="9" t="n">
+        <v>43903</v>
+      </c>
+      <c r="AI11" s="10" t="n">
+        <v>43894</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1288,10 +1394,16 @@
       <c r="AC12" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH12" s="9" t="n">
+        <v>43900</v>
+      </c>
+      <c r="AI12" s="10" t="n">
+        <v>43901</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -1350,10 +1462,16 @@
       <c r="AC13" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH13" s="9" t="n">
+        <v>43911</v>
+      </c>
+      <c r="AI13" s="10" t="n">
+        <v>43907</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -1412,10 +1530,16 @@
       <c r="AC14" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH14" s="9" t="n">
+        <v>43908</v>
+      </c>
+      <c r="AI14" s="10" t="n">
+        <v>43903</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1474,10 +1598,16 @@
       <c r="AC15" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH15" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI15" s="10" t="n">
+        <v>43899</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1557,10 +1687,16 @@
       <c r="AC16" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="AH16" s="9" t="n">
+        <v>43891</v>
+      </c>
+      <c r="AI16" s="10" t="n">
+        <v>43890</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1619,10 +1755,16 @@
       <c r="AC17" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH17" s="9" t="n">
+        <v>43900</v>
+      </c>
+      <c r="AI17" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -1696,10 +1838,16 @@
       <c r="AC18" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="AH18" s="9" t="n">
+        <v>43888</v>
+      </c>
+      <c r="AI18" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1764,10 +1912,16 @@
       <c r="AC19" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH19" s="9" t="n">
+        <v>43911</v>
+      </c>
+      <c r="AI19" s="10" t="n">
+        <v>43901</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -1835,10 +1989,16 @@
       <c r="AC20" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH20" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI20" s="10" t="n">
+        <v>43906</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -1906,10 +2066,16 @@
       <c r="AC21" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH21" s="9" t="n">
+        <v>43905</v>
+      </c>
+      <c r="AI21" s="10" t="n">
+        <v>43905</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -1992,10 +2158,16 @@
       <c r="AC22" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="AH22" s="9" t="n">
+        <v>43887</v>
+      </c>
+      <c r="AI22" s="10" t="n">
+        <v>43885</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -2063,10 +2235,16 @@
       <c r="AC23" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH23" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI23" s="10" t="n">
+        <v>43896</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -2149,10 +2327,16 @@
       <c r="AG24" s="0" t="n">
         <v>0.3155</v>
       </c>
+      <c r="AH24" s="9" t="n">
+        <v>43903</v>
+      </c>
+      <c r="AI24" s="10" t="n">
+        <v>43894</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -2238,10 +2422,16 @@
       <c r="AG25" s="0" t="n">
         <v>30079.4932</v>
       </c>
+      <c r="AH25" s="9" t="n">
+        <v>43884</v>
+      </c>
+      <c r="AI25" s="10" t="n">
+        <v>43894</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -2309,10 +2499,16 @@
       <c r="AC26" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH26" s="9" t="n">
+        <v>43882</v>
+      </c>
+      <c r="AI26" s="10" t="n">
+        <v>43836</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -2392,10 +2588,16 @@
       <c r="AG27" s="0" t="n">
         <v>79719.7898</v>
       </c>
+      <c r="AH27" s="9" t="n">
+        <v>43882</v>
+      </c>
+      <c r="AI27" s="10" t="n">
+        <v>43866</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -2463,10 +2665,16 @@
       <c r="AC28" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH28" s="9" t="n">
+        <v>43909</v>
+      </c>
+      <c r="AI28" s="10" t="n">
+        <v>43906</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -2525,10 +2733,16 @@
       <c r="AC29" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH29" s="9" t="n">
+        <v>43912</v>
+      </c>
+      <c r="AI29" s="10" t="n">
+        <v>43906</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -2608,10 +2822,16 @@
       <c r="AG30" s="0" t="n">
         <v>157176.2658</v>
       </c>
+      <c r="AH30" s="9" t="n">
+        <v>43896</v>
+      </c>
+      <c r="AI30" s="10" t="n">
+        <v>43902</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2682,10 +2902,16 @@
       <c r="AG31" s="0" t="n">
         <v>48762.3895</v>
       </c>
+      <c r="AH31" s="9" t="n">
+        <v>43896</v>
+      </c>
+      <c r="AI31" s="10" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2747,10 +2973,16 @@
       <c r="AC32" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH32" s="9" t="n">
+        <v>43907</v>
+      </c>
+      <c r="AI32" s="10" t="n">
+        <v>43902</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2821,10 +3053,16 @@
       <c r="AG33" s="0" t="n">
         <v>152000</v>
       </c>
+      <c r="AH33" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI33" s="10" t="n">
+        <v>43901</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2892,10 +3130,16 @@
       <c r="AC34" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH34" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI34" s="10" t="n">
+        <v>43898</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2969,10 +3213,16 @@
       <c r="AG35" s="0" t="n">
         <v>31461.9423</v>
       </c>
+      <c r="AH35" s="9" t="n">
+        <v>43903</v>
+      </c>
+      <c r="AI35" s="10" t="n">
+        <v>43903</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -3040,10 +3290,16 @@
       <c r="AC36" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH36" s="9" t="n">
+        <v>43904</v>
+      </c>
+      <c r="AI36" s="10" t="n">
+        <v>43906</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -3102,10 +3358,16 @@
       <c r="AC37" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH37" s="9" t="n">
+        <v>43907</v>
+      </c>
+      <c r="AI37" s="10" t="n">
+        <v>43904</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -3191,10 +3453,16 @@
       <c r="AG38" s="0" t="n">
         <v>1644.5779</v>
       </c>
+      <c r="AH38" s="9" t="n">
+        <v>43892</v>
+      </c>
+      <c r="AI38" s="10" t="n">
+        <v>43899</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -3265,10 +3533,16 @@
       <c r="AC39" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="AH39" s="9" t="n">
+        <v>43896</v>
+      </c>
+      <c r="AI39" s="10" t="n">
+        <v>43902</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -3354,10 +3628,16 @@
       <c r="AG40" s="0" t="n">
         <v>16.6454</v>
       </c>
+      <c r="AH40" s="9" t="n">
+        <v>43895</v>
+      </c>
+      <c r="AI40" s="10" t="n">
+        <v>43889</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -3440,10 +3720,16 @@
       <c r="AC41" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="AH41" s="9" t="n">
+        <v>43909</v>
+      </c>
+      <c r="AI41" s="10" t="n">
+        <v>43906</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -3523,10 +3809,13 @@
       <c r="AG42" s="0" t="n">
         <v>1406472.4</v>
       </c>
+      <c r="AH42" s="9" t="n">
+        <v>43893</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -3605,6 +3894,12 @@
       </c>
       <c r="AC43" s="0" t="n">
         <v>66</v>
+      </c>
+      <c r="AH43" s="9" t="n">
+        <v>43895</v>
+      </c>
+      <c r="AI43" s="10" t="n">
+        <v>43906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>